<commit_message>
Added aluminum polymer to BOM
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Part</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>P100KDBCT-ND</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>P16405CT-ND</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,73 +645,71 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.58899999999999997</v>
+      </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.11033</v>
-      </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4">
-        <v>1.0999999999999999E-2</v>
+        <v>0.62</v>
       </c>
       <c r="E9" s="4">
-        <v>2.0400000000000001E-3</v>
+        <v>0.11033</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4">
-        <v>0.43</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E10" s="4">
-        <v>6.0139999999999999E-2</v>
+        <v>2.0400000000000001E-3</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4">
         <v>0.43</v>
@@ -717,13 +721,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4">
         <v>0.43</v>
@@ -734,138 +738,155 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.43</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6.0139999999999999E-2</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.29699999999999999</v>
-      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="4">
-        <v>1.6719999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="E15" s="4">
-        <v>1.657</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4">
-        <v>3.762</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="E16" s="4">
-        <v>1.6830000000000001</v>
+        <v>1.657</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="4">
-        <v>1.89</v>
+        <v>3.762</v>
       </c>
       <c r="E17" s="4">
-        <v>1.44</v>
+        <v>1.6830000000000001</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.89</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.44</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D19" s="4">
         <v>0.499</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="4">
         <v>0.21174999999999999</v>
       </c>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8">
-        <f>SUMPRODUCT($B3:$B20,D3:D20)</f>
-        <v>18.601000000000003</v>
-      </c>
-      <c r="E22" s="8">
-        <f>SUMPRODUCT($B3:$B20,E3:E20)</f>
-        <v>7.8102099999999988</v>
-      </c>
-      <c r="F22" s="4"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8">
+        <f>SUMPRODUCT($B3:$B21,D3:D21)</f>
+        <v>19.590000000000003</v>
+      </c>
+      <c r="E23" s="8">
+        <f>SUMPRODUCT($B3:$B21,E3:E21)</f>
+        <v>8.3992100000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BOM updates, added 1% calculation
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="0.1% accurate" sheetId="1" r:id="rId1"/>
+    <sheet name="1% accurate" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Part</t>
   </si>
@@ -81,9 +81,6 @@
     <t>2.2uF</t>
   </si>
   <si>
-    <t>296-20899-1-ND</t>
-  </si>
-  <si>
     <t>MAX11612EUA+-ND</t>
   </si>
   <si>
@@ -130,6 +127,21 @@
   </si>
   <si>
     <t>Cost %</t>
+  </si>
+  <si>
+    <t>LM4040AIM3-2.5/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT20KCT-ND</t>
+  </si>
+  <si>
+    <t>576-1047-1-ND</t>
   </si>
 </sst>
 </file>
@@ -138,9 +150,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +182,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -215,7 +233,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -239,7 +257,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -542,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,10 +574,11 @@
     <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -569,16 +589,17 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -596,10 +617,11 @@
       </c>
       <c r="F3" s="9">
         <f>B3*E3/$E$23</f>
-        <v>3.0002821693945027E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>2.8307577556584262E-3</v>
+      </c>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -616,11 +638,12 @@
         <v>7.62E-3</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" ref="F4:F21" si="0">B4*E4/$E$23</f>
-        <v>3.6289127191723985E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <f>B4*E4/$E$23</f>
+        <v>3.4238689044630492E-3</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -637,11 +660,12 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="F5" s="9">
-        <f t="shared" si="0"/>
-        <v>1.9287528231821801E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <f>B5*E5/$E$23</f>
+        <v>1.819772842923274E-3</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -658,19 +682,20 @@
         <v>2.4750000000000001E-2</v>
       </c>
       <c r="F6" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1786822808335547E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <f>B6*E6/$E$23</f>
+        <v>1.1120834040086675E-2</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D7" s="4">
         <v>0.98899999999999999</v>
@@ -679,14 +704,16 @@
         <v>0.58899999999999997</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" si="0"/>
-        <v>7.0125642768784205E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <f>B7*E7/$E$23</f>
+        <v>6.6163345955667183E-2</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -694,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4">
         <v>0.62</v>
@@ -703,11 +730,12 @@
         <v>0.11033</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="0"/>
-        <v>1.3135759196400613E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <f>B9*E9/$E$23</f>
+        <v>1.2393551713563261E-2</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -715,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4">
         <v>1.0999999999999999E-2</v>
@@ -724,11 +752,12 @@
         <v>2.0400000000000001E-3</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="0"/>
-        <v>7.2863995542437926E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <f>B10*E10/$E$23</f>
+        <v>6.8746974065990354E-4</v>
+      </c>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -736,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4">
         <v>0.43</v>
@@ -745,11 +774,12 @@
         <v>6.0139999999999999E-2</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="0"/>
-        <v>7.1601972090232294E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <f>B11*E11/$E$23</f>
+        <v>6.7556258502102281E-3</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -757,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="4">
         <v>0.43</v>
@@ -766,11 +796,12 @@
         <v>6.0139999999999999E-2</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="0"/>
-        <v>5.7281577672185835E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <f>B12*E12/$E$23</f>
+        <v>5.4045006801681825E-2</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -778,7 +809,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4">
         <v>0.43</v>
@@ -787,37 +818,40 @@
         <v>6.0139999999999999E-2</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="0"/>
-        <v>5.7281577672185835E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <f>B13*E13/$E$23</f>
+        <v>5.4045006801681825E-2</v>
+      </c>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>21</v>
+      <c r="C15" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="4">
-        <v>0.65</v>
+        <v>1.76</v>
       </c>
       <c r="E15" s="4">
-        <v>0.29699999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" si="0"/>
-        <v>3.5360468425006633E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <f>B15*E15/$E$23</f>
+        <v>8.9865325576457988E-2</v>
+      </c>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -825,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4">
         <v>1.6719999999999999</v>
@@ -834,11 +868,12 @@
         <v>1.657</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="0"/>
-        <v>0.19728045851931314</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <f>B16*E16/$E$23</f>
+        <v>0.18613355560023859</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -846,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="4">
         <v>3.762</v>
@@ -855,11 +890,12 @@
         <v>1.6830000000000001</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="0"/>
-        <v>0.20037598774170429</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <f>B17*E17/$E$23</f>
+        <v>0.18905417868147348</v>
+      </c>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -867,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="4">
         <v>1.89</v>
@@ -876,11 +912,12 @@
         <v>1.44</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" si="0"/>
-        <v>0.17144469539397156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <f>B18*E18/$E$23</f>
+        <v>0.16175758603762436</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -888,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4">
         <v>0.499</v>
@@ -897,18 +934,20 @@
         <v>0.21174999999999999</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="0"/>
-        <v>5.0421408680102052E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <f>B19*E19/$E$23</f>
+        <v>4.7572456727037443E-2</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -920,26 +959,24 @@
         <v>1</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" si="0"/>
-        <v>0.11905881624581359</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
+        <f>B21*E21/$E$23</f>
+        <v>0.11233165697057247</v>
+      </c>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7">
         <f>SUMPRODUCT($B3:$B21,D3:D21)</f>
-        <v>19.590000000000003</v>
+        <v>20.700000000000003</v>
       </c>
       <c r="E23" s="7">
         <f>SUMPRODUCT($B3:$B21,E3:E21)</f>
-        <v>8.3992100000000001</v>
+        <v>8.9022100000000002</v>
       </c>
     </row>
   </sheetData>
@@ -950,12 +987,433 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.3E-3</v>
+      </c>
+      <c r="F3" s="9">
+        <f>B3*E3/$E$23</f>
+        <v>3.7223977559259244E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E4" s="4">
+        <v>7.62E-3</v>
+      </c>
+      <c r="F4" s="9">
+        <f>B4*E4/$E$23</f>
+        <v>4.5023287143104041E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F5" s="9">
+        <f>B5*E5/$E$23</f>
+        <v>2.3929699859523796E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.4750000000000001E-2</v>
+      </c>
+      <c r="F6" s="9">
+        <f>B6*E6/$E$23</f>
+        <v>1.4623705469708989E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="F7" s="9">
+        <f>B7*E7/$E$23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.11033</v>
+      </c>
+      <c r="F9" s="9">
+        <f>B9*E9/$E$23</f>
+        <v>1.6297307317909016E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.0400000000000001E-3</v>
+      </c>
+      <c r="F10" s="9">
+        <f>B10*E10/$E$23</f>
+        <v>9.0401088358201031E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F11" s="9">
+        <f>B11*E11/$E$23</f>
+        <v>5.9085678665490859E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F12" s="9">
+        <f>B12*E12/$E$23</f>
+        <v>4.7268542932392688E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F13" s="9">
+        <f>B13*E13/$E$23</f>
+        <v>4.7268542932392688E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="F15" s="9">
+        <f>B15*E15/$E$23</f>
+        <v>3.1167695496046428E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.657</v>
+      </c>
+      <c r="F16" s="9">
+        <f>B16*E16/$E$23</f>
+        <v>0.24476242387179592</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3.762</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.6830000000000001</v>
+      </c>
+      <c r="F17" s="9">
+        <f>B17*E17/$E$23</f>
+        <v>0.24860299298505281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.89</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.44</v>
+      </c>
+      <c r="F18" s="9">
+        <f>B18*E18/$E$23</f>
+        <v>0.21270844319576709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.499</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.21174999999999999</v>
+      </c>
+      <c r="F19" s="9">
+        <f>B19*E19/$E$23</f>
+        <v>6.2556962287088444E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <f>B21*E21/$E$23</f>
+        <v>0.14771419666372715</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7">
+        <f>SUMPRODUCT($B3:$B21,D3:D21)</f>
+        <v>11.565999999999999</v>
+      </c>
+      <c r="E23" s="7">
+        <f>SUMPRODUCT($B3:$B21,E3:E21)</f>
+        <v>6.7698299999999998</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>